<commit_message>
Added a window to enter test information Fixed all icons on color theme switch Added help window
</commit_message>
<xml_diff>
--- a/src/tools/TestReportModel.xlsx
+++ b/src/tools/TestReportModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\repos\VVToolkit\src\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0732D740-9877-4F1A-B70D-F46E18A5CC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B99A391-20BE-42CC-8C82-4AE26789AB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{44A9439D-9982-41D3-B9B3-8E8D971FADF8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>VERIFICATION FILE REPORT</t>
   </si>
@@ -160,12 +160,6 @@
   </si>
   <si>
     <t>&lt;item.result[0].output&gt;</t>
-  </si>
-  <si>
-    <t>A10:B25</t>
-  </si>
-  <si>
-    <t>A26:B33</t>
   </si>
   <si>
     <t>&lt;iterationNumber+1&gt;/&lt;item.repetitions&gt;</t>
@@ -188,6 +182,45 @@
       </rPr>
       <t xml:space="preserve"> &lt;item.wasTestRepeated&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>VFR Author:</t>
+  </si>
+  <si>
+    <t>A11:B26</t>
+  </si>
+  <si>
+    <t>A27:B34</t>
+  </si>
+  <si>
+    <t>VFR data block:</t>
+  </si>
+  <si>
+    <t>A3:B8</t>
+  </si>
+  <si>
+    <t>&lt;testFields.name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;testFields.project&gt;</t>
+  </si>
+  <si>
+    <t>&lt;testFields.date&gt;</t>
+  </si>
+  <si>
+    <t>&lt;testFields.author&gt;</t>
+  </si>
+  <si>
+    <t>&lt;testFields.conductor&gt;</t>
+  </si>
+  <si>
+    <t>&lt;testFields.testCount&gt;</t>
+  </si>
+  <si>
+    <t>Delete area:</t>
+  </si>
+  <si>
+    <t>C1:D5</t>
   </si>
 </sst>
 </file>
@@ -372,81 +405,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,261 +798,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5645569-F519-4890-BE22-5440213D30AB}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" style="6" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="26"/>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="16"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="24"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="11"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="24"/>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="B29" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="B30" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="17"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="B31" s="15"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B32" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="26"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="16"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added highlights to excel Added delta times for executions Cool loading circle animation :)
</commit_message>
<xml_diff>
--- a/src/tools/TestReportModel.xlsx
+++ b/src/tools/TestReportModel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\repos\VVToolkit\src\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B99A391-20BE-42CC-8C82-4AE26789AB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C0464F-BEDD-4BDF-9059-2FE9983EC305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{44A9439D-9982-41D3-B9B3-8E8D971FADF8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>VERIFICATION FILE REPORT</t>
   </si>
@@ -99,9 +99,6 @@
     <t>&lt;item.runcode&gt;</t>
   </si>
   <si>
-    <t>&lt;item.testResult&gt;</t>
-  </si>
-  <si>
     <t>Justification:</t>
   </si>
   <si>
@@ -135,18 +132,12 @@
     <t>Iteration block:</t>
   </si>
   <si>
-    <t>&lt;iteration.result&gt;</t>
-  </si>
-  <si>
     <t>&lt;item.validationCmd.resultToString(iteration.result)&gt;</t>
   </si>
   <si>
     <t>&lt;iteration.returnCode&gt;</t>
   </si>
   <si>
-    <t>&lt;iteration.executionTime&gt;</t>
-  </si>
-  <si>
     <t>&lt;iteration.output&gt;</t>
   </si>
   <si>
@@ -156,9 +147,6 @@
     <t>&lt;item.result[0].returnCode&gt;</t>
   </si>
   <si>
-    <t>&lt;item.result[0].executionTime&gt;</t>
-  </si>
-  <si>
     <t>&lt;item.result[0].output&gt;</t>
   </si>
   <si>
@@ -168,31 +156,9 @@
     <t>&lt;itemNumber+1&gt;/&lt;totalTestCount&gt;</t>
   </si>
   <si>
-    <r>
-      <t>Number of test repetitions:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;item.wasTestRepeated&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>VFR Author:</t>
   </si>
   <si>
-    <t>A11:B26</t>
-  </si>
-  <si>
-    <t>A27:B34</t>
-  </si>
-  <si>
     <t>VFR data block:</t>
   </si>
   <si>
@@ -221,6 +187,54 @@
   </si>
   <si>
     <t>C1:D5</t>
+  </si>
+  <si>
+    <t>Sample return code:</t>
+  </si>
+  <si>
+    <t>Sample execution time:</t>
+  </si>
+  <si>
+    <t>Sample output:</t>
+  </si>
+  <si>
+    <t>&lt;TestResult.toString(item.testResult)&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;TestResult.toString(iteration.result)&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;TestResult.toExcelColor(item.testResult)&gt;</t>
+  </si>
+  <si>
+    <t>&lt;TestResult.toExcelColor(iteration.result)&gt;</t>
+  </si>
+  <si>
+    <t>A11:C25</t>
+  </si>
+  <si>
+    <t>&lt;"green" if item.wasTestRepeated == 0 else "red"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;"This test was not repeated." if item.wasTestRepeated == 0 else f"This test was repeated {item.wasTestRepeated} time(s)."&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iteration.timeOfExecution&gt;</t>
+  </si>
+  <si>
+    <t>Delta of execution:</t>
+  </si>
+  <si>
+    <t>&lt;iteration.deltaOfExecution(testFields.date)&gt;</t>
+  </si>
+  <si>
+    <t>A26:C34</t>
+  </si>
+  <si>
+    <t>&lt;iteration.executionTime&gt; s</t>
+  </si>
+  <si>
+    <t>&lt;item.result[0].executionTime&gt; s</t>
   </si>
 </sst>
 </file>
@@ -282,9 +296,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,75 +418,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -481,15 +473,178 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -800,290 +955,340 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5645569-F519-4890-BE22-5440213D30AB}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="18" style="7" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="18"/>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C6" s="26"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="C7" s="26"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="26"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="26"/>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="26"/>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="26"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="26"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="26"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="26"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="26"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="26"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="26"/>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="26"/>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="26"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="26"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="26"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="26"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="26"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="26"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="26"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="26"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="26"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="26"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="26"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="26"/>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="16"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="24"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="21"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="15"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="C34" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A10:B10"/>
   </mergeCells>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>EXACT(C1,"yellow")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5">
+      <formula>EXACT(C1,"red")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="6">
+      <formula>EXACT(C1,"green")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>